<commit_message>
Integrate Agora data for bldgs/SYCEU, cost-outputs/DR, fuels/MPIiFE, fuels/MPIiFI, and fuels/MPIiFP
</commit_message>
<xml_diff>
--- a/InputData/cost-outputs/DR/Discount Rate.xlsx
+++ b/InputData/cost-outputs/DR/Discount Rate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\cost-outputs\DR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\cost-outputs\DR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2C3EA9-E3B0-4ECF-849E-A2873623A600}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="23955" windowHeight="13605"/>
+    <workbookView xWindow="39390" yWindow="5370" windowWidth="14940" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -46,15 +47,9 @@
     <t>Page 17, Table A1</t>
   </si>
   <si>
-    <t>of Social Cost of Carbon (in the SCoC variable), as well as the discount rate built into the health</t>
-  </si>
-  <si>
     <t>damages values in the SCoHIbP Social Cost of Health Impacts by Pollutant variable.</t>
   </si>
   <si>
-    <t>We choose to use a 3% discount rate here, for consistency with the 3% rate used for the central estimate</t>
-  </si>
-  <si>
     <t>This is the annual percentage rate by which future savings (e.g. fuel cost savings) are discounted when</t>
   </si>
   <si>
@@ -71,12 +66,18 @@
   </si>
   <si>
     <t>Annual Perc (dimensionless)</t>
+  </si>
+  <si>
+    <t>We choose to use a 3% discount rate here, for consistency with the discount rate built into the health</t>
+  </si>
+  <si>
+    <t>However, note that the EU's Social Cost of Carbon (SCoC) variable uses an estimate based on a 1% discount rate.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,6 +228,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -262,6 +280,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,21 +472,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -459,74 +494,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" location="8" display="http://www.whitehouse.gov/omb/circulars_a094#8"/>
+    <hyperlink ref="B6" r:id="rId1" location="8" display="http://www.whitehouse.gov/omb/circulars_a094#8" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -534,7 +569,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -544,18 +579,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.86328125" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>

</xml_diff>